<commit_message>
fix demo data sheet name
</commit_message>
<xml_diff>
--- a/chapter3/input/chapter3_demo_data.xlsx
+++ b/chapter3/input/chapter3_demo_data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\副業関連\独立\workdir\practical-mi-guide\chapter3\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E397AE-C02D-46D4-8923-8F7D66AA4BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE19C14-A254-4B7A-A9CC-7DC93E144C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="890" yWindow="2680" windowWidth="34540" windowHeight="17720" activeTab="6" xr2:uid="{AFFCA931-CB2A-4AED-B7E5-2638B5FCE6AD}"/>
+    <workbookView xWindow="1050" yWindow="3050" windowWidth="29720" windowHeight="17720" xr2:uid="{AFFCA931-CB2A-4AED-B7E5-2638B5FCE6AD}"/>
   </bookViews>
   <sheets>
     <sheet name="初期データ" sheetId="2" r:id="rId1"/>
-    <sheet name="整形Step1" sheetId="4" r:id="rId2"/>
-    <sheet name="整形Step2" sheetId="5" r:id="rId3"/>
-    <sheet name="整形Step3" sheetId="6" r:id="rId4"/>
+    <sheet name="整形処理1" sheetId="4" r:id="rId2"/>
+    <sheet name="整形処理2" sheetId="5" r:id="rId3"/>
+    <sheet name="整形処理3" sheetId="6" r:id="rId4"/>
     <sheet name="整形後" sheetId="7" r:id="rId5"/>
     <sheet name="ヒートマップ" sheetId="8" r:id="rId6"/>
     <sheet name="元データ" sheetId="1" r:id="rId7"/>
@@ -1157,6 +1157,24 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1173,24 +1191,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2581,7 +2581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29A7775-745C-46D9-8F8E-94D6562DAC1D}">
   <dimension ref="B5:AJ36"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
@@ -2717,103 +2717,103 @@
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="77">
+      <c r="D6" s="83">
         <v>45310</v>
       </c>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="79"/>
-      <c r="I6" s="77">
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="83">
         <v>45321</v>
       </c>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="78"/>
-      <c r="N6" s="78"/>
-      <c r="O6" s="78">
+      <c r="J6" s="84"/>
+      <c r="K6" s="84"/>
+      <c r="L6" s="84"/>
+      <c r="M6" s="84"/>
+      <c r="N6" s="84"/>
+      <c r="O6" s="84">
         <v>45329</v>
       </c>
-      <c r="P6" s="78"/>
-      <c r="Q6" s="79"/>
-      <c r="R6" s="77">
+      <c r="P6" s="84"/>
+      <c r="Q6" s="85"/>
+      <c r="R6" s="83">
         <v>45337</v>
       </c>
-      <c r="S6" s="78"/>
-      <c r="T6" s="78"/>
-      <c r="U6" s="79"/>
-      <c r="V6" s="77">
+      <c r="S6" s="84"/>
+      <c r="T6" s="84"/>
+      <c r="U6" s="85"/>
+      <c r="V6" s="83">
         <v>45350</v>
       </c>
-      <c r="W6" s="78"/>
-      <c r="X6" s="78"/>
-      <c r="Y6" s="79"/>
-      <c r="Z6" s="77">
+      <c r="W6" s="84"/>
+      <c r="X6" s="84"/>
+      <c r="Y6" s="85"/>
+      <c r="Z6" s="83">
         <v>45366</v>
       </c>
-      <c r="AA6" s="78"/>
-      <c r="AB6" s="78"/>
-      <c r="AC6" s="79"/>
-      <c r="AD6" s="77">
+      <c r="AA6" s="84"/>
+      <c r="AB6" s="84"/>
+      <c r="AC6" s="85"/>
+      <c r="AD6" s="83">
         <v>45392</v>
       </c>
-      <c r="AE6" s="78"/>
-      <c r="AF6" s="78"/>
-      <c r="AG6" s="78"/>
-      <c r="AH6" s="78"/>
-      <c r="AI6" s="78"/>
-      <c r="AJ6" s="79"/>
+      <c r="AE6" s="84"/>
+      <c r="AF6" s="84"/>
+      <c r="AG6" s="84"/>
+      <c r="AH6" s="84"/>
+      <c r="AI6" s="84"/>
+      <c r="AJ6" s="85"/>
     </row>
     <row r="7" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="80" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="80" t="s">
+      <c r="D7" s="86" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="87"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="81"/>
-      <c r="K7" s="81"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="81"/>
-      <c r="N7" s="81"/>
-      <c r="O7" s="81"/>
-      <c r="P7" s="81"/>
-      <c r="Q7" s="82"/>
-      <c r="R7" s="80" t="s">
-        <v>40</v>
-      </c>
-      <c r="S7" s="81"/>
-      <c r="T7" s="81"/>
-      <c r="U7" s="82"/>
-      <c r="V7" s="80" t="s">
+      <c r="J7" s="87"/>
+      <c r="K7" s="87"/>
+      <c r="L7" s="87"/>
+      <c r="M7" s="87"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="87"/>
+      <c r="P7" s="87"/>
+      <c r="Q7" s="88"/>
+      <c r="R7" s="86" t="s">
+        <v>40</v>
+      </c>
+      <c r="S7" s="87"/>
+      <c r="T7" s="87"/>
+      <c r="U7" s="88"/>
+      <c r="V7" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="W7" s="81"/>
-      <c r="X7" s="81"/>
-      <c r="Y7" s="82"/>
-      <c r="Z7" s="80" t="s">
+      <c r="W7" s="87"/>
+      <c r="X7" s="87"/>
+      <c r="Y7" s="88"/>
+      <c r="Z7" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="AA7" s="81"/>
-      <c r="AB7" s="81"/>
-      <c r="AC7" s="82"/>
-      <c r="AD7" s="80" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE7" s="81"/>
-      <c r="AF7" s="81"/>
-      <c r="AG7" s="81"/>
-      <c r="AH7" s="81"/>
-      <c r="AI7" s="81"/>
-      <c r="AJ7" s="82"/>
+      <c r="AA7" s="87"/>
+      <c r="AB7" s="87"/>
+      <c r="AC7" s="88"/>
+      <c r="AD7" s="86" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE7" s="87"/>
+      <c r="AF7" s="87"/>
+      <c r="AG7" s="87"/>
+      <c r="AH7" s="87"/>
+      <c r="AI7" s="87"/>
+      <c r="AJ7" s="88"/>
     </row>
     <row r="8" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="1" t="s">
@@ -4476,34 +4476,34 @@
       <c r="C25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="83" t="s">
+      <c r="D25" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="E25" s="84"/>
-      <c r="F25" s="84"/>
-      <c r="G25" s="84"/>
-      <c r="H25" s="84"/>
-      <c r="I25" s="84"/>
-      <c r="J25" s="84"/>
-      <c r="K25" s="84"/>
-      <c r="L25" s="84"/>
-      <c r="M25" s="84"/>
-      <c r="N25" s="84"/>
-      <c r="O25" s="84"/>
-      <c r="P25" s="84"/>
-      <c r="Q25" s="84"/>
-      <c r="R25" s="84"/>
-      <c r="S25" s="84"/>
-      <c r="T25" s="84"/>
-      <c r="U25" s="84"/>
-      <c r="V25" s="84"/>
-      <c r="W25" s="84"/>
-      <c r="X25" s="84"/>
-      <c r="Y25" s="84"/>
-      <c r="Z25" s="84"/>
-      <c r="AA25" s="84"/>
-      <c r="AB25" s="84"/>
-      <c r="AC25" s="85"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="78"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="78"/>
+      <c r="I25" s="78"/>
+      <c r="J25" s="78"/>
+      <c r="K25" s="78"/>
+      <c r="L25" s="78"/>
+      <c r="M25" s="78"/>
+      <c r="N25" s="78"/>
+      <c r="O25" s="78"/>
+      <c r="P25" s="78"/>
+      <c r="Q25" s="78"/>
+      <c r="R25" s="78"/>
+      <c r="S25" s="78"/>
+      <c r="T25" s="78"/>
+      <c r="U25" s="78"/>
+      <c r="V25" s="78"/>
+      <c r="W25" s="78"/>
+      <c r="X25" s="78"/>
+      <c r="Y25" s="78"/>
+      <c r="Z25" s="78"/>
+      <c r="AA25" s="78"/>
+      <c r="AB25" s="78"/>
+      <c r="AC25" s="79"/>
       <c r="AD25" s="8">
         <v>9.8199999999999985</v>
       </c>
@@ -4641,65 +4641,65 @@
       <c r="C28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="86" t="s">
+      <c r="D28" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="E28" s="87"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
-      <c r="H28" s="87"/>
-      <c r="I28" s="87"/>
-      <c r="J28" s="87"/>
-      <c r="K28" s="87"/>
-      <c r="L28" s="87"/>
-      <c r="M28" s="87"/>
-      <c r="N28" s="87"/>
-      <c r="O28" s="87"/>
-      <c r="P28" s="87"/>
-      <c r="Q28" s="88"/>
-      <c r="R28" s="86" t="s">
+      <c r="E28" s="81"/>
+      <c r="F28" s="81"/>
+      <c r="G28" s="81"/>
+      <c r="H28" s="81"/>
+      <c r="I28" s="81"/>
+      <c r="J28" s="81"/>
+      <c r="K28" s="81"/>
+      <c r="L28" s="81"/>
+      <c r="M28" s="81"/>
+      <c r="N28" s="81"/>
+      <c r="O28" s="81"/>
+      <c r="P28" s="81"/>
+      <c r="Q28" s="82"/>
+      <c r="R28" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="S28" s="87"/>
-      <c r="T28" s="87"/>
-      <c r="U28" s="87"/>
-      <c r="V28" s="87"/>
-      <c r="W28" s="87"/>
-      <c r="X28" s="87"/>
-      <c r="Y28" s="87"/>
-      <c r="Z28" s="87"/>
-      <c r="AA28" s="87"/>
-      <c r="AB28" s="87"/>
-      <c r="AC28" s="87"/>
-      <c r="AD28" s="87"/>
-      <c r="AE28" s="87"/>
-      <c r="AF28" s="87"/>
-      <c r="AG28" s="87"/>
-      <c r="AH28" s="87"/>
-      <c r="AI28" s="87"/>
-      <c r="AJ28" s="88"/>
+      <c r="S28" s="81"/>
+      <c r="T28" s="81"/>
+      <c r="U28" s="81"/>
+      <c r="V28" s="81"/>
+      <c r="W28" s="81"/>
+      <c r="X28" s="81"/>
+      <c r="Y28" s="81"/>
+      <c r="Z28" s="81"/>
+      <c r="AA28" s="81"/>
+      <c r="AB28" s="81"/>
+      <c r="AC28" s="81"/>
+      <c r="AD28" s="81"/>
+      <c r="AE28" s="81"/>
+      <c r="AF28" s="81"/>
+      <c r="AG28" s="81"/>
+      <c r="AH28" s="81"/>
+      <c r="AI28" s="81"/>
+      <c r="AJ28" s="82"/>
     </row>
     <row r="29" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="21"/>
       <c r="C29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="86" t="s">
+      <c r="D29" s="80" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="87"/>
-      <c r="F29" s="87"/>
-      <c r="G29" s="87"/>
-      <c r="H29" s="87"/>
-      <c r="I29" s="87"/>
-      <c r="J29" s="87"/>
-      <c r="K29" s="87"/>
-      <c r="L29" s="87"/>
-      <c r="M29" s="87"/>
-      <c r="N29" s="87"/>
-      <c r="O29" s="87"/>
-      <c r="P29" s="87"/>
-      <c r="Q29" s="88"/>
+      <c r="E29" s="81"/>
+      <c r="F29" s="81"/>
+      <c r="G29" s="81"/>
+      <c r="H29" s="81"/>
+      <c r="I29" s="81"/>
+      <c r="J29" s="81"/>
+      <c r="K29" s="81"/>
+      <c r="L29" s="81"/>
+      <c r="M29" s="81"/>
+      <c r="N29" s="81"/>
+      <c r="O29" s="81"/>
+      <c r="P29" s="81"/>
+      <c r="Q29" s="82"/>
       <c r="R29" s="47">
         <v>100</v>
       </c>
@@ -4763,22 +4763,22 @@
       <c r="C30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="86" t="s">
+      <c r="D30" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="87"/>
-      <c r="F30" s="87"/>
-      <c r="G30" s="87"/>
-      <c r="H30" s="87"/>
-      <c r="I30" s="87"/>
-      <c r="J30" s="87"/>
-      <c r="K30" s="87"/>
-      <c r="L30" s="87"/>
-      <c r="M30" s="87"/>
-      <c r="N30" s="87"/>
-      <c r="O30" s="87"/>
-      <c r="P30" s="87"/>
-      <c r="Q30" s="88"/>
+      <c r="E30" s="81"/>
+      <c r="F30" s="81"/>
+      <c r="G30" s="81"/>
+      <c r="H30" s="81"/>
+      <c r="I30" s="81"/>
+      <c r="J30" s="81"/>
+      <c r="K30" s="81"/>
+      <c r="L30" s="81"/>
+      <c r="M30" s="81"/>
+      <c r="N30" s="81"/>
+      <c r="O30" s="81"/>
+      <c r="P30" s="81"/>
+      <c r="Q30" s="82"/>
       <c r="R30" s="47">
         <v>0.01</v>
       </c>
@@ -5330,17 +5330,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="D25:AC25"/>
-    <mergeCell ref="D30:Q30"/>
-    <mergeCell ref="D29:Q29"/>
-    <mergeCell ref="D28:Q28"/>
-    <mergeCell ref="R28:AJ28"/>
-    <mergeCell ref="V6:Y6"/>
-    <mergeCell ref="Z6:AC6"/>
-    <mergeCell ref="AD6:AJ6"/>
-    <mergeCell ref="V7:Y7"/>
-    <mergeCell ref="Z7:AC7"/>
-    <mergeCell ref="AD7:AJ7"/>
     <mergeCell ref="D6:H6"/>
     <mergeCell ref="R6:U6"/>
     <mergeCell ref="D7:H7"/>
@@ -5348,6 +5337,17 @@
     <mergeCell ref="R7:U7"/>
     <mergeCell ref="I6:N6"/>
     <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="V6:Y6"/>
+    <mergeCell ref="Z6:AC6"/>
+    <mergeCell ref="AD6:AJ6"/>
+    <mergeCell ref="V7:Y7"/>
+    <mergeCell ref="Z7:AC7"/>
+    <mergeCell ref="AD7:AJ7"/>
+    <mergeCell ref="D25:AC25"/>
+    <mergeCell ref="D30:Q30"/>
+    <mergeCell ref="D29:Q29"/>
+    <mergeCell ref="D28:Q28"/>
+    <mergeCell ref="R28:AJ28"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18654,7 +18654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFD9269-7F18-4E64-8D48-3C1F1E4D91C0}">
   <dimension ref="B2:AF47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" topLeftCell="M1" activePane="topRight" state="frozen"/>
       <selection pane="topRight"/>
     </sheetView>

</xml_diff>

<commit_message>
fix demo data DP021
</commit_message>
<xml_diff>
--- a/chapter3/input/chapter3_demo_data.xlsx
+++ b/chapter3/input/chapter3_demo_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\副業関連\独立\workdir\practical-mi-guide\chapter3\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE19C14-A254-4B7A-A9CC-7DC93E144C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104C61A9-DD08-48E9-92BE-976B5749AC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="3050" windowWidth="29720" windowHeight="17720" xr2:uid="{AFFCA931-CB2A-4AED-B7E5-2638B5FCE6AD}"/>
+    <workbookView xWindow="7370" yWindow="500" windowWidth="29720" windowHeight="17720" activeTab="4" xr2:uid="{AFFCA931-CB2A-4AED-B7E5-2638B5FCE6AD}"/>
   </bookViews>
   <sheets>
     <sheet name="初期データ" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="整形処理2" sheetId="5" r:id="rId3"/>
     <sheet name="整形処理3" sheetId="6" r:id="rId4"/>
     <sheet name="整形後" sheetId="7" r:id="rId5"/>
-    <sheet name="ヒートマップ" sheetId="8" r:id="rId6"/>
+    <sheet name="ヒートマップ" sheetId="9" r:id="rId6"/>
     <sheet name="元データ" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="136">
   <si>
     <t>サンプル作成日</t>
     <rPh sb="4" eb="7">
@@ -687,8 +687,46 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>材料１</t>
+  </si>
+  <si>
+    <t>材料２</t>
+  </si>
+  <si>
+    <t>材料３</t>
+  </si>
+  <si>
+    <t>材料４</t>
+  </si>
+  <si>
+    <t>材料５</t>
+  </si>
+  <si>
+    <t>材料６</t>
+  </si>
+  <si>
+    <t>材料７</t>
+  </si>
+  <si>
+    <t>材料８</t>
+  </si>
+  <si>
+    <t>材料９</t>
+  </si>
+  <si>
+    <t>材料１０</t>
+  </si>
+  <si>
+    <t>材料１１</t>
+  </si>
+  <si>
+    <t>材料１２</t>
+  </si>
+  <si>
+    <t>材料１３</t>
+  </si>
+  <si>
     <t>耐擦過性</t>
-    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -925,7 +963,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1139,18 +1177,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1191,6 +1217,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2581,8 +2616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29A7775-745C-46D9-8F8E-94D6562DAC1D}">
   <dimension ref="B5:AJ36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="8" topLeftCell="U9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight"/>
@@ -2717,103 +2752,103 @@
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="83">
+      <c r="D6" s="79">
         <v>45310</v>
       </c>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="83">
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="81"/>
+      <c r="I6" s="79">
         <v>45321</v>
       </c>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
-      <c r="L6" s="84"/>
-      <c r="M6" s="84"/>
-      <c r="N6" s="84"/>
-      <c r="O6" s="84">
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="80"/>
+      <c r="N6" s="80"/>
+      <c r="O6" s="80">
         <v>45329</v>
       </c>
-      <c r="P6" s="84"/>
-      <c r="Q6" s="85"/>
-      <c r="R6" s="83">
+      <c r="P6" s="80"/>
+      <c r="Q6" s="81"/>
+      <c r="R6" s="79">
         <v>45337</v>
       </c>
-      <c r="S6" s="84"/>
-      <c r="T6" s="84"/>
-      <c r="U6" s="85"/>
-      <c r="V6" s="83">
+      <c r="S6" s="80"/>
+      <c r="T6" s="80"/>
+      <c r="U6" s="81"/>
+      <c r="V6" s="79">
         <v>45350</v>
       </c>
-      <c r="W6" s="84"/>
-      <c r="X6" s="84"/>
-      <c r="Y6" s="85"/>
-      <c r="Z6" s="83">
+      <c r="W6" s="80"/>
+      <c r="X6" s="80"/>
+      <c r="Y6" s="81"/>
+      <c r="Z6" s="79">
         <v>45366</v>
       </c>
-      <c r="AA6" s="84"/>
-      <c r="AB6" s="84"/>
-      <c r="AC6" s="85"/>
-      <c r="AD6" s="83">
+      <c r="AA6" s="80"/>
+      <c r="AB6" s="80"/>
+      <c r="AC6" s="81"/>
+      <c r="AD6" s="79">
         <v>45392</v>
       </c>
-      <c r="AE6" s="84"/>
-      <c r="AF6" s="84"/>
-      <c r="AG6" s="84"/>
-      <c r="AH6" s="84"/>
-      <c r="AI6" s="84"/>
-      <c r="AJ6" s="85"/>
+      <c r="AE6" s="80"/>
+      <c r="AF6" s="80"/>
+      <c r="AG6" s="80"/>
+      <c r="AH6" s="80"/>
+      <c r="AI6" s="80"/>
+      <c r="AJ6" s="81"/>
     </row>
     <row r="7" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="86" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="86" t="s">
+      <c r="D7" s="82" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="87"/>
-      <c r="K7" s="87"/>
-      <c r="L7" s="87"/>
-      <c r="M7" s="87"/>
-      <c r="N7" s="87"/>
-      <c r="O7" s="87"/>
-      <c r="P7" s="87"/>
-      <c r="Q7" s="88"/>
-      <c r="R7" s="86" t="s">
-        <v>40</v>
-      </c>
-      <c r="S7" s="87"/>
-      <c r="T7" s="87"/>
-      <c r="U7" s="88"/>
-      <c r="V7" s="86" t="s">
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="83"/>
+      <c r="M7" s="83"/>
+      <c r="N7" s="83"/>
+      <c r="O7" s="83"/>
+      <c r="P7" s="83"/>
+      <c r="Q7" s="84"/>
+      <c r="R7" s="82" t="s">
+        <v>40</v>
+      </c>
+      <c r="S7" s="83"/>
+      <c r="T7" s="83"/>
+      <c r="U7" s="84"/>
+      <c r="V7" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="W7" s="87"/>
-      <c r="X7" s="87"/>
-      <c r="Y7" s="88"/>
-      <c r="Z7" s="86" t="s">
+      <c r="W7" s="83"/>
+      <c r="X7" s="83"/>
+      <c r="Y7" s="84"/>
+      <c r="Z7" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="AA7" s="87"/>
-      <c r="AB7" s="87"/>
-      <c r="AC7" s="88"/>
-      <c r="AD7" s="86" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE7" s="87"/>
-      <c r="AF7" s="87"/>
-      <c r="AG7" s="87"/>
-      <c r="AH7" s="87"/>
-      <c r="AI7" s="87"/>
-      <c r="AJ7" s="88"/>
+      <c r="AA7" s="83"/>
+      <c r="AB7" s="83"/>
+      <c r="AC7" s="84"/>
+      <c r="AD7" s="82" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE7" s="83"/>
+      <c r="AF7" s="83"/>
+      <c r="AG7" s="83"/>
+      <c r="AH7" s="83"/>
+      <c r="AI7" s="83"/>
+      <c r="AJ7" s="84"/>
     </row>
     <row r="8" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="1" t="s">
@@ -4476,34 +4511,34 @@
       <c r="C25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="77" t="s">
+      <c r="D25" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="E25" s="78"/>
-      <c r="F25" s="78"/>
-      <c r="G25" s="78"/>
-      <c r="H25" s="78"/>
-      <c r="I25" s="78"/>
-      <c r="J25" s="78"/>
-      <c r="K25" s="78"/>
-      <c r="L25" s="78"/>
-      <c r="M25" s="78"/>
-      <c r="N25" s="78"/>
-      <c r="O25" s="78"/>
-      <c r="P25" s="78"/>
-      <c r="Q25" s="78"/>
-      <c r="R25" s="78"/>
-      <c r="S25" s="78"/>
-      <c r="T25" s="78"/>
-      <c r="U25" s="78"/>
-      <c r="V25" s="78"/>
-      <c r="W25" s="78"/>
-      <c r="X25" s="78"/>
-      <c r="Y25" s="78"/>
-      <c r="Z25" s="78"/>
-      <c r="AA25" s="78"/>
-      <c r="AB25" s="78"/>
-      <c r="AC25" s="79"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="74"/>
+      <c r="J25" s="74"/>
+      <c r="K25" s="74"/>
+      <c r="L25" s="74"/>
+      <c r="M25" s="74"/>
+      <c r="N25" s="74"/>
+      <c r="O25" s="74"/>
+      <c r="P25" s="74"/>
+      <c r="Q25" s="74"/>
+      <c r="R25" s="74"/>
+      <c r="S25" s="74"/>
+      <c r="T25" s="74"/>
+      <c r="U25" s="74"/>
+      <c r="V25" s="74"/>
+      <c r="W25" s="74"/>
+      <c r="X25" s="74"/>
+      <c r="Y25" s="74"/>
+      <c r="Z25" s="74"/>
+      <c r="AA25" s="74"/>
+      <c r="AB25" s="74"/>
+      <c r="AC25" s="75"/>
       <c r="AD25" s="8">
         <v>9.8199999999999985</v>
       </c>
@@ -4641,65 +4676,65 @@
       <c r="C28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="80" t="s">
+      <c r="D28" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="E28" s="81"/>
-      <c r="F28" s="81"/>
-      <c r="G28" s="81"/>
-      <c r="H28" s="81"/>
-      <c r="I28" s="81"/>
-      <c r="J28" s="81"/>
-      <c r="K28" s="81"/>
-      <c r="L28" s="81"/>
-      <c r="M28" s="81"/>
-      <c r="N28" s="81"/>
-      <c r="O28" s="81"/>
-      <c r="P28" s="81"/>
-      <c r="Q28" s="82"/>
-      <c r="R28" s="80" t="s">
+      <c r="E28" s="77"/>
+      <c r="F28" s="77"/>
+      <c r="G28" s="77"/>
+      <c r="H28" s="77"/>
+      <c r="I28" s="77"/>
+      <c r="J28" s="77"/>
+      <c r="K28" s="77"/>
+      <c r="L28" s="77"/>
+      <c r="M28" s="77"/>
+      <c r="N28" s="77"/>
+      <c r="O28" s="77"/>
+      <c r="P28" s="77"/>
+      <c r="Q28" s="78"/>
+      <c r="R28" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="S28" s="81"/>
-      <c r="T28" s="81"/>
-      <c r="U28" s="81"/>
-      <c r="V28" s="81"/>
-      <c r="W28" s="81"/>
-      <c r="X28" s="81"/>
-      <c r="Y28" s="81"/>
-      <c r="Z28" s="81"/>
-      <c r="AA28" s="81"/>
-      <c r="AB28" s="81"/>
-      <c r="AC28" s="81"/>
-      <c r="AD28" s="81"/>
-      <c r="AE28" s="81"/>
-      <c r="AF28" s="81"/>
-      <c r="AG28" s="81"/>
-      <c r="AH28" s="81"/>
-      <c r="AI28" s="81"/>
-      <c r="AJ28" s="82"/>
+      <c r="S28" s="77"/>
+      <c r="T28" s="77"/>
+      <c r="U28" s="77"/>
+      <c r="V28" s="77"/>
+      <c r="W28" s="77"/>
+      <c r="X28" s="77"/>
+      <c r="Y28" s="77"/>
+      <c r="Z28" s="77"/>
+      <c r="AA28" s="77"/>
+      <c r="AB28" s="77"/>
+      <c r="AC28" s="77"/>
+      <c r="AD28" s="77"/>
+      <c r="AE28" s="77"/>
+      <c r="AF28" s="77"/>
+      <c r="AG28" s="77"/>
+      <c r="AH28" s="77"/>
+      <c r="AI28" s="77"/>
+      <c r="AJ28" s="78"/>
     </row>
     <row r="29" spans="2:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="21"/>
       <c r="C29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="80" t="s">
+      <c r="D29" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="81"/>
-      <c r="F29" s="81"/>
-      <c r="G29" s="81"/>
-      <c r="H29" s="81"/>
-      <c r="I29" s="81"/>
-      <c r="J29" s="81"/>
-      <c r="K29" s="81"/>
-      <c r="L29" s="81"/>
-      <c r="M29" s="81"/>
-      <c r="N29" s="81"/>
-      <c r="O29" s="81"/>
-      <c r="P29" s="81"/>
-      <c r="Q29" s="82"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="77"/>
+      <c r="G29" s="77"/>
+      <c r="H29" s="77"/>
+      <c r="I29" s="77"/>
+      <c r="J29" s="77"/>
+      <c r="K29" s="77"/>
+      <c r="L29" s="77"/>
+      <c r="M29" s="77"/>
+      <c r="N29" s="77"/>
+      <c r="O29" s="77"/>
+      <c r="P29" s="77"/>
+      <c r="Q29" s="78"/>
       <c r="R29" s="47">
         <v>100</v>
       </c>
@@ -4763,22 +4798,22 @@
       <c r="C30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="80" t="s">
+      <c r="D30" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="81"/>
-      <c r="F30" s="81"/>
-      <c r="G30" s="81"/>
-      <c r="H30" s="81"/>
-      <c r="I30" s="81"/>
-      <c r="J30" s="81"/>
-      <c r="K30" s="81"/>
-      <c r="L30" s="81"/>
-      <c r="M30" s="81"/>
-      <c r="N30" s="81"/>
-      <c r="O30" s="81"/>
-      <c r="P30" s="81"/>
-      <c r="Q30" s="82"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="77"/>
+      <c r="H30" s="77"/>
+      <c r="I30" s="77"/>
+      <c r="J30" s="77"/>
+      <c r="K30" s="77"/>
+      <c r="L30" s="77"/>
+      <c r="M30" s="77"/>
+      <c r="N30" s="77"/>
+      <c r="O30" s="77"/>
+      <c r="P30" s="77"/>
+      <c r="Q30" s="78"/>
       <c r="R30" s="47">
         <v>0.01</v>
       </c>
@@ -4798,7 +4833,7 @@
         <v>0.03</v>
       </c>
       <c r="X30" s="47">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="Y30" s="47">
         <v>0.03</v>
@@ -5359,7 +5394,7 @@
   <dimension ref="B5:AJ36"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="U9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight"/>
@@ -7845,7 +7880,7 @@
         <v>0.03</v>
       </c>
       <c r="X30" s="47">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="Y30" s="47">
         <v>0.03</v>
@@ -10282,7 +10317,7 @@
         <v>100</v>
       </c>
       <c r="Y27" s="38">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="Z27" s="24" t="s">
         <v>60</v>
@@ -11318,7 +11353,7 @@
   <dimension ref="B5:AD39"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="5" ySplit="5" topLeftCell="O6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="5" topLeftCell="O11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight"/>
@@ -13245,7 +13280,7 @@
         <v>100</v>
       </c>
       <c r="Z27" s="38">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="AA27" s="24" t="s">
         <v>60</v>
@@ -14306,8 +14341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC155531-539F-473A-BEFE-FAB0C4C3EE43}">
   <dimension ref="B4:AD39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="I12" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <pane xSplit="5" ySplit="3" topLeftCell="P11" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="E4" sqref="E4"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
@@ -16176,7 +16211,7 @@
         <v>100</v>
       </c>
       <c r="V27" s="38">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="W27" s="30">
         <v>10</v>
@@ -17235,1406 +17270,1387 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946DA809-6F7B-4F40-B49B-27E3855F241E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{378FCD36-4939-467E-95CA-2D9070DB49FB}">
   <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.4140625" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="21" max="24" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.75" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="72"/>
-      <c r="B1" s="72" t="s">
-        <v>96</v>
-      </c>
-      <c r="C1" s="72" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" s="72" t="s">
-        <v>98</v>
-      </c>
-      <c r="E1" s="72" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" s="72" t="s">
-        <v>100</v>
-      </c>
-      <c r="G1" s="72" t="s">
-        <v>101</v>
-      </c>
-      <c r="H1" s="72" t="s">
-        <v>102</v>
-      </c>
-      <c r="I1" s="72" t="s">
-        <v>103</v>
-      </c>
-      <c r="J1" s="72" t="s">
-        <v>104</v>
-      </c>
-      <c r="K1" s="72" t="s">
-        <v>105</v>
-      </c>
-      <c r="L1" s="72" t="s">
-        <v>106</v>
-      </c>
-      <c r="M1" s="72" t="s">
-        <v>107</v>
-      </c>
-      <c r="N1" s="72" t="s">
-        <v>108</v>
-      </c>
-      <c r="O1" s="72" t="s">
+      <c r="A1" s="87"/>
+      <c r="B1" s="87" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="87" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="87" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="87" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="87" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="87" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="87" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="87" t="s">
+        <v>129</v>
+      </c>
+      <c r="J1" s="87" t="s">
+        <v>130</v>
+      </c>
+      <c r="K1" s="87" t="s">
+        <v>131</v>
+      </c>
+      <c r="L1" s="87" t="s">
+        <v>132</v>
+      </c>
+      <c r="M1" s="87" t="s">
+        <v>133</v>
+      </c>
+      <c r="N1" s="87" t="s">
+        <v>134</v>
+      </c>
+      <c r="O1" s="87" t="s">
         <v>86</v>
       </c>
-      <c r="P1" s="72" t="s">
+      <c r="P1" s="87" t="s">
         <v>87</v>
       </c>
-      <c r="Q1" s="72" t="s">
+      <c r="Q1" s="87" t="s">
         <v>88</v>
       </c>
-      <c r="R1" s="72" t="s">
+      <c r="R1" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="S1" s="72" t="s">
+      <c r="S1" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="T1" s="72" t="s">
+      <c r="T1" s="87" t="s">
         <v>91</v>
       </c>
-      <c r="U1" s="72" t="s">
+      <c r="U1" s="87" t="s">
+        <v>135</v>
+      </c>
+      <c r="V1" s="87" t="s">
+        <v>92</v>
+      </c>
+      <c r="W1" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="X1" s="87" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y1" s="87" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="85" t="s">
         <v>122</v>
       </c>
-      <c r="V1" s="72" t="s">
+      <c r="B2" s="85">
+        <v>1</v>
+      </c>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="85"/>
+      <c r="U2" s="85"/>
+      <c r="V2" s="85"/>
+      <c r="W2" s="85"/>
+      <c r="X2" s="85"/>
+      <c r="Y2" s="85"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="85" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="85">
+        <v>0.54532269214902873</v>
+      </c>
+      <c r="C3" s="85">
+        <v>1</v>
+      </c>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="85"/>
+      <c r="R3" s="85"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="85"/>
+      <c r="U3" s="85"/>
+      <c r="V3" s="85"/>
+      <c r="W3" s="85"/>
+      <c r="X3" s="85"/>
+      <c r="Y3" s="85"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="85" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="85">
+        <v>-0.5693038369307919</v>
+      </c>
+      <c r="C4" s="85">
+        <v>-0.99796012768573961</v>
+      </c>
+      <c r="D4" s="85">
+        <v>1</v>
+      </c>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="85"/>
+      <c r="Q4" s="85"/>
+      <c r="R4" s="85"/>
+      <c r="S4" s="85"/>
+      <c r="T4" s="85"/>
+      <c r="U4" s="85"/>
+      <c r="V4" s="85"/>
+      <c r="W4" s="85"/>
+      <c r="X4" s="85"/>
+      <c r="Y4" s="85"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="85" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="85">
+        <v>0.37186951414850039</v>
+      </c>
+      <c r="C5" s="85">
+        <v>0.78685883447847571</v>
+      </c>
+      <c r="D5" s="85">
+        <v>-0.78525374292679184</v>
+      </c>
+      <c r="E5" s="85">
+        <v>1</v>
+      </c>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="85"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="85"/>
+      <c r="S5" s="85"/>
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="85"/>
+      <c r="X5" s="85"/>
+      <c r="Y5" s="85"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="85" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="85">
+        <v>-0.52142976010762865</v>
+      </c>
+      <c r="C6" s="85">
+        <v>-0.80214333130506021</v>
+      </c>
+      <c r="D6" s="85">
+        <v>0.80050706133146232</v>
+      </c>
+      <c r="E6" s="85">
+        <v>-0.81378476241257014</v>
+      </c>
+      <c r="F6" s="85">
+        <v>1</v>
+      </c>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
+      <c r="L6" s="85"/>
+      <c r="M6" s="85"/>
+      <c r="N6" s="85"/>
+      <c r="O6" s="85"/>
+      <c r="P6" s="85"/>
+      <c r="Q6" s="85"/>
+      <c r="R6" s="85"/>
+      <c r="S6" s="85"/>
+      <c r="T6" s="85"/>
+      <c r="U6" s="85"/>
+      <c r="V6" s="85"/>
+      <c r="W6" s="85"/>
+      <c r="X6" s="85"/>
+      <c r="Y6" s="85"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="85" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="85">
+        <v>-0.40937219968250366</v>
+      </c>
+      <c r="C7" s="85">
+        <v>-0.24062558079337174</v>
+      </c>
+      <c r="D7" s="85">
+        <v>0.24013473533300858</v>
+      </c>
+      <c r="E7" s="85">
+        <v>-0.17615657920993991</v>
+      </c>
+      <c r="F7" s="85">
+        <v>0.21844348946250985</v>
+      </c>
+      <c r="G7" s="85">
+        <v>1</v>
+      </c>
+      <c r="H7" s="85"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="85"/>
+      <c r="K7" s="85"/>
+      <c r="L7" s="85"/>
+      <c r="M7" s="85"/>
+      <c r="N7" s="85"/>
+      <c r="O7" s="85"/>
+      <c r="P7" s="85"/>
+      <c r="Q7" s="85"/>
+      <c r="R7" s="85"/>
+      <c r="S7" s="85"/>
+      <c r="T7" s="85"/>
+      <c r="U7" s="85"/>
+      <c r="V7" s="85"/>
+      <c r="W7" s="85"/>
+      <c r="X7" s="85"/>
+      <c r="Y7" s="85"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="85" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="85">
+        <v>0.2064701282579329</v>
+      </c>
+      <c r="C8" s="85">
+        <v>0.13363062095621231</v>
+      </c>
+      <c r="D8" s="85">
+        <v>-0.13335803155218626</v>
+      </c>
+      <c r="E8" s="85">
+        <v>9.7827974015615812E-2</v>
+      </c>
+      <c r="F8" s="85">
+        <v>-0.1213118698538683</v>
+      </c>
+      <c r="G8" s="85">
+        <v>-0.59150144445301611</v>
+      </c>
+      <c r="H8" s="85">
+        <v>1</v>
+      </c>
+      <c r="I8" s="85"/>
+      <c r="J8" s="85"/>
+      <c r="K8" s="85"/>
+      <c r="L8" s="85"/>
+      <c r="M8" s="85"/>
+      <c r="N8" s="85"/>
+      <c r="O8" s="85"/>
+      <c r="P8" s="85"/>
+      <c r="Q8" s="85"/>
+      <c r="R8" s="85"/>
+      <c r="S8" s="85"/>
+      <c r="T8" s="85"/>
+      <c r="U8" s="85"/>
+      <c r="V8" s="85"/>
+      <c r="W8" s="85"/>
+      <c r="X8" s="85"/>
+      <c r="Y8" s="85"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="85" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="85">
+        <v>0.2064701282579329</v>
+      </c>
+      <c r="C9" s="85">
+        <v>0.13363062095621234</v>
+      </c>
+      <c r="D9" s="85">
+        <v>-0.13335803155218626</v>
+      </c>
+      <c r="E9" s="85">
+        <v>9.7827974015615812E-2</v>
+      </c>
+      <c r="F9" s="85">
+        <v>-0.1213118698538683</v>
+      </c>
+      <c r="G9" s="85">
+        <v>-0.59150144445301611</v>
+      </c>
+      <c r="H9" s="85">
+        <v>-3.1250000000000097E-2</v>
+      </c>
+      <c r="I9" s="85">
+        <v>1</v>
+      </c>
+      <c r="J9" s="85"/>
+      <c r="K9" s="85"/>
+      <c r="L9" s="85"/>
+      <c r="M9" s="85"/>
+      <c r="N9" s="85"/>
+      <c r="O9" s="85"/>
+      <c r="P9" s="85"/>
+      <c r="Q9" s="85"/>
+      <c r="R9" s="85"/>
+      <c r="S9" s="85"/>
+      <c r="T9" s="85"/>
+      <c r="U9" s="85"/>
+      <c r="V9" s="85"/>
+      <c r="W9" s="85"/>
+      <c r="X9" s="85"/>
+      <c r="Y9" s="85"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="85" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" s="85">
+        <v>4.7941143432472522E-2</v>
+      </c>
+      <c r="C10" s="85">
+        <v>0.1689159811730441</v>
+      </c>
+      <c r="D10" s="85">
+        <v>-0.16857141413961296</v>
+      </c>
+      <c r="E10" s="85">
+        <v>0.15141990995385896</v>
+      </c>
+      <c r="F10" s="85">
+        <v>-0.12657001882882701</v>
+      </c>
+      <c r="G10" s="85">
+        <v>-4.0645506075046016E-2</v>
+      </c>
+      <c r="H10" s="85">
+        <v>2.2572347453581727E-2</v>
+      </c>
+      <c r="I10" s="85">
+        <v>2.2572347453581727E-2</v>
+      </c>
+      <c r="J10" s="85">
+        <v>1</v>
+      </c>
+      <c r="K10" s="85"/>
+      <c r="L10" s="85"/>
+      <c r="M10" s="85"/>
+      <c r="N10" s="85"/>
+      <c r="O10" s="85"/>
+      <c r="P10" s="85"/>
+      <c r="Q10" s="85"/>
+      <c r="R10" s="85"/>
+      <c r="S10" s="85"/>
+      <c r="T10" s="85"/>
+      <c r="U10" s="85"/>
+      <c r="V10" s="85"/>
+      <c r="W10" s="85"/>
+      <c r="X10" s="85"/>
+      <c r="Y10" s="85"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="85" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" s="85">
+        <v>-0.42354601289696908</v>
+      </c>
+      <c r="C11" s="85">
+        <v>-0.46770717334674256</v>
+      </c>
+      <c r="D11" s="85">
+        <v>0.46675311043265155</v>
+      </c>
+      <c r="E11" s="85">
+        <v>-0.41926274578121053</v>
+      </c>
+      <c r="F11" s="85">
+        <v>0.35045651291117474</v>
+      </c>
+      <c r="G11" s="85">
+        <v>0.11254231022778623</v>
+      </c>
+      <c r="H11" s="85">
+        <v>-6.2500000000000042E-2</v>
+      </c>
+      <c r="I11" s="85">
+        <v>-6.2500000000000042E-2</v>
+      </c>
+      <c r="J11" s="85">
+        <v>-0.7674598134217786</v>
+      </c>
+      <c r="K11" s="85">
+        <v>1</v>
+      </c>
+      <c r="L11" s="85"/>
+      <c r="M11" s="85"/>
+      <c r="N11" s="85"/>
+      <c r="O11" s="85"/>
+      <c r="P11" s="85"/>
+      <c r="Q11" s="85"/>
+      <c r="R11" s="85"/>
+      <c r="S11" s="85"/>
+      <c r="T11" s="85"/>
+      <c r="U11" s="85"/>
+      <c r="V11" s="85"/>
+      <c r="W11" s="85"/>
+      <c r="X11" s="85"/>
+      <c r="Y11" s="85"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="85" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" s="85">
+        <v>-0.56094629067505208</v>
+      </c>
+      <c r="C12" s="85">
+        <v>-0.48279450151921821</v>
+      </c>
+      <c r="D12" s="85">
+        <v>0.481809662382092</v>
+      </c>
+      <c r="E12" s="85">
+        <v>-0.3534430028951282</v>
+      </c>
+      <c r="F12" s="85">
+        <v>0.43828804592365272</v>
+      </c>
+      <c r="G12" s="85">
+        <v>0.27591017991328259</v>
+      </c>
+      <c r="H12" s="85">
+        <v>-0.15322580645161285</v>
+      </c>
+      <c r="I12" s="85">
+        <v>-0.15322580645161291</v>
+      </c>
+      <c r="J12" s="85">
+        <v>-8.1551706929069462E-2</v>
+      </c>
+      <c r="K12" s="85">
+        <v>0.22580645161290325</v>
+      </c>
+      <c r="L12" s="85">
+        <v>1</v>
+      </c>
+      <c r="M12" s="85"/>
+      <c r="N12" s="85"/>
+      <c r="O12" s="85"/>
+      <c r="P12" s="85"/>
+      <c r="Q12" s="85"/>
+      <c r="R12" s="85"/>
+      <c r="S12" s="85"/>
+      <c r="T12" s="85"/>
+      <c r="U12" s="85"/>
+      <c r="V12" s="85"/>
+      <c r="W12" s="85"/>
+      <c r="X12" s="85"/>
+      <c r="Y12" s="85"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="85" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" s="85">
+        <v>5.4122225092713113E-3</v>
+      </c>
+      <c r="C13" s="85">
+        <v>0.22252462162536571</v>
+      </c>
+      <c r="D13" s="85">
+        <v>-0.22207069981047078</v>
+      </c>
+      <c r="E13" s="85">
+        <v>0.1629052738543682</v>
+      </c>
+      <c r="F13" s="85">
+        <v>-0.20201116888279116</v>
+      </c>
+      <c r="G13" s="85">
+        <v>9.3703953559000658E-2</v>
+      </c>
+      <c r="H13" s="85">
+        <v>-5.2038180890226576E-2</v>
+      </c>
+      <c r="I13" s="85">
+        <v>-5.2038180890226576E-2</v>
+      </c>
+      <c r="J13" s="85">
+        <v>3.7587964797009037E-2</v>
+      </c>
+      <c r="K13" s="85">
+        <v>-0.10407636178045325</v>
+      </c>
+      <c r="L13" s="85">
+        <v>-0.6983188145269128</v>
+      </c>
+      <c r="M13" s="85">
+        <v>1</v>
+      </c>
+      <c r="N13" s="85"/>
+      <c r="O13" s="85"/>
+      <c r="P13" s="85"/>
+      <c r="Q13" s="85"/>
+      <c r="R13" s="85"/>
+      <c r="S13" s="85"/>
+      <c r="T13" s="85"/>
+      <c r="U13" s="85"/>
+      <c r="V13" s="85"/>
+      <c r="W13" s="85"/>
+      <c r="X13" s="85"/>
+      <c r="Y13" s="85"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="85" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="85">
+        <v>6.8298341815840067E-15</v>
+      </c>
+      <c r="C14" s="85">
+        <v>1.0443996526137254E-16</v>
+      </c>
+      <c r="D14" s="85">
+        <v>-1.0422692106773353E-16</v>
+      </c>
+      <c r="E14" s="85">
+        <v>1.5603704304785335E-17</v>
+      </c>
+      <c r="F14" s="85">
+        <v>-1.6554503680555037E-16</v>
+      </c>
+      <c r="G14" s="85">
+        <v>2.9587283593366958E-16</v>
+      </c>
+      <c r="H14" s="85">
+        <v>-6.9781887052612257E-17</v>
+      </c>
+      <c r="I14" s="85">
+        <v>-6.9781887052612257E-17</v>
+      </c>
+      <c r="J14" s="85">
+        <v>-2.3690120647793115E-16</v>
+      </c>
+      <c r="K14" s="85">
+        <v>0</v>
+      </c>
+      <c r="L14" s="85">
+        <v>-2.9713577712725213E-16</v>
+      </c>
+      <c r="M14" s="85">
+        <v>1.3072760860698715E-16</v>
+      </c>
+      <c r="N14" s="85">
+        <v>1</v>
+      </c>
+      <c r="O14" s="85"/>
+      <c r="P14" s="85"/>
+      <c r="Q14" s="85"/>
+      <c r="R14" s="85"/>
+      <c r="S14" s="85"/>
+      <c r="T14" s="85"/>
+      <c r="U14" s="85"/>
+      <c r="V14" s="85"/>
+      <c r="W14" s="85"/>
+      <c r="X14" s="85"/>
+      <c r="Y14" s="85"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="85" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C15" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D15" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E15" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F15" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G15" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H15" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I15" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J15" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K15" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L15" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M15" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N15" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O15" s="85">
+        <v>1</v>
+      </c>
+      <c r="P15" s="85"/>
+      <c r="Q15" s="85"/>
+      <c r="R15" s="85"/>
+      <c r="S15" s="85"/>
+      <c r="T15" s="85"/>
+      <c r="U15" s="85"/>
+      <c r="V15" s="85"/>
+      <c r="W15" s="85"/>
+      <c r="X15" s="85"/>
+      <c r="Y15" s="85"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="85" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="85">
+        <v>-0.63644724213007908</v>
+      </c>
+      <c r="C16" s="85">
+        <v>-0.64888568452304984</v>
+      </c>
+      <c r="D16" s="85">
+        <v>0.64756204058007127</v>
+      </c>
+      <c r="E16" s="85">
+        <v>-0.47503462477680736</v>
+      </c>
+      <c r="F16" s="85">
+        <v>0.58906809792264891</v>
+      </c>
+      <c r="G16" s="85">
+        <v>0.37082892492880132</v>
+      </c>
+      <c r="H16" s="85">
+        <v>-0.20593861776197844</v>
+      </c>
+      <c r="I16" s="85">
+        <v>-0.20593861776197844</v>
+      </c>
+      <c r="J16" s="85">
+        <v>-0.10960716207035329</v>
+      </c>
+      <c r="K16" s="85">
+        <v>0.30348848933344197</v>
+      </c>
+      <c r="L16" s="85">
+        <v>0.74403629643037428</v>
+      </c>
+      <c r="M16" s="85">
+        <v>-0.34293347338819458</v>
+      </c>
+      <c r="N16" s="85">
+        <v>-2.3598342282655199E-16</v>
+      </c>
+      <c r="O16" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P16" s="85">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="85"/>
+      <c r="R16" s="85"/>
+      <c r="S16" s="85"/>
+      <c r="T16" s="85"/>
+      <c r="U16" s="85"/>
+      <c r="V16" s="85"/>
+      <c r="W16" s="85"/>
+      <c r="X16" s="85"/>
+      <c r="Y16" s="85"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="85" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="85">
+        <v>-0.63090569434588195</v>
+      </c>
+      <c r="C17" s="85">
+        <v>-0.64323583518874972</v>
+      </c>
+      <c r="D17" s="85">
+        <v>0.64192371621700783</v>
+      </c>
+      <c r="E17" s="85">
+        <v>-0.47089849706960152</v>
+      </c>
+      <c r="F17" s="85">
+        <v>0.58393908046967202</v>
+      </c>
+      <c r="G17" s="85">
+        <v>0.3676001165198311</v>
+      </c>
+      <c r="H17" s="85">
+        <v>-0.20414550968420586</v>
+      </c>
+      <c r="I17" s="85">
+        <v>-0.20414550968420586</v>
+      </c>
+      <c r="J17" s="85">
+        <v>-0.10865281222657011</v>
+      </c>
+      <c r="K17" s="85">
+        <v>0.3008460142714614</v>
+      </c>
+      <c r="L17" s="85">
+        <v>0.73755797047197014</v>
+      </c>
+      <c r="M17" s="85">
+        <v>-0.339947550747975</v>
+      </c>
+      <c r="N17" s="85">
+        <v>-2.1497449050234554E-16</v>
+      </c>
+      <c r="O17" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P17" s="85">
+        <v>0.99129299741224342</v>
+      </c>
+      <c r="Q17" s="85">
+        <v>1</v>
+      </c>
+      <c r="R17" s="85"/>
+      <c r="S17" s="85"/>
+      <c r="T17" s="85"/>
+      <c r="U17" s="85"/>
+      <c r="V17" s="85"/>
+      <c r="W17" s="85"/>
+      <c r="X17" s="85"/>
+      <c r="Y17" s="85"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="85" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="85">
+        <v>-0.23585737871463944</v>
+      </c>
+      <c r="C18" s="85">
+        <v>-0.56694670951384141</v>
+      </c>
+      <c r="D18" s="85">
+        <v>0.56495355180761331</v>
+      </c>
+      <c r="E18" s="85">
+        <v>-0.35888261168794822</v>
+      </c>
+      <c r="F18" s="85">
+        <v>0.48462175706697358</v>
+      </c>
+      <c r="G18" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H18" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I18" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J18" s="85">
+        <v>-7.3308961400745887E-2</v>
+      </c>
+      <c r="K18" s="85">
+        <v>0.21174738846497995</v>
+      </c>
+      <c r="L18" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M18" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N18" s="85">
+        <v>1.6525460586108752E-15</v>
+      </c>
+      <c r="O18" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P18" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q18" s="85">
+        <v>0</v>
+      </c>
+      <c r="R18" s="85">
+        <v>1</v>
+      </c>
+      <c r="S18" s="85"/>
+      <c r="T18" s="85"/>
+      <c r="U18" s="85"/>
+      <c r="V18" s="85"/>
+      <c r="W18" s="85"/>
+      <c r="X18" s="85"/>
+      <c r="Y18" s="85"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="85" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C19" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D19" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E19" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F19" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G19" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H19" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J19" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K19" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L19" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M19" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N19" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O19" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P19" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q19" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R19" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S19" s="85">
+        <v>1</v>
+      </c>
+      <c r="T19" s="85"/>
+      <c r="U19" s="85"/>
+      <c r="V19" s="85"/>
+      <c r="W19" s="85"/>
+      <c r="X19" s="85"/>
+      <c r="Y19" s="85"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="85" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C20" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D20" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E20" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F20" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G20" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H20" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I20" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J20" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K20" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L20" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M20" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N20" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O20" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P20" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q20" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R20" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S20" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T20" s="85">
+        <v>1</v>
+      </c>
+      <c r="U20" s="85"/>
+      <c r="V20" s="85"/>
+      <c r="W20" s="85"/>
+      <c r="X20" s="85"/>
+      <c r="Y20" s="85"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="85" t="s">
+        <v>135</v>
+      </c>
+      <c r="B21" s="85">
+        <v>-0.65684655212468779</v>
+      </c>
+      <c r="C21" s="85">
+        <v>-0.74501977471698688</v>
+      </c>
+      <c r="D21" s="85">
+        <v>0.74350002950496497</v>
+      </c>
+      <c r="E21" s="85">
+        <v>-0.54541223142273476</v>
+      </c>
+      <c r="F21" s="85">
+        <v>0.67634005815658671</v>
+      </c>
+      <c r="G21" s="85">
+        <v>0.30504180067972075</v>
+      </c>
+      <c r="H21" s="85">
+        <v>-0.15636742794798861</v>
+      </c>
+      <c r="I21" s="85">
+        <v>-0.15636742794798861</v>
+      </c>
+      <c r="J21" s="85">
+        <v>-0.12584574623964012</v>
+      </c>
+      <c r="K21" s="85">
+        <v>0.34845109292030901</v>
+      </c>
+      <c r="L21" s="85">
+        <v>0.76338890244138069</v>
+      </c>
+      <c r="M21" s="85">
+        <v>-0.38484971956554048</v>
+      </c>
+      <c r="N21" s="85">
+        <v>2.2613484572857596E-16</v>
+      </c>
+      <c r="O21" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P21" s="85">
+        <v>0.78920382806196909</v>
+      </c>
+      <c r="Q21" s="85">
+        <v>0.79023941466963321</v>
+      </c>
+      <c r="R21" s="85">
+        <v>0.99387189842671075</v>
+      </c>
+      <c r="S21" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T21" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U21" s="85">
+        <v>1</v>
+      </c>
+      <c r="V21" s="85"/>
+      <c r="W21" s="85"/>
+      <c r="X21" s="85"/>
+      <c r="Y21" s="85"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="85" t="s">
         <v>92</v>
       </c>
-      <c r="W1" s="72" t="s">
+      <c r="B22" s="85">
+        <v>-0.6139086961176804</v>
+      </c>
+      <c r="C22" s="85">
+        <v>-0.5947704002421923</v>
+      </c>
+      <c r="D22" s="85">
+        <v>0.59355714456939646</v>
+      </c>
+      <c r="E22" s="85">
+        <v>-0.55235314072510733</v>
+      </c>
+      <c r="F22" s="85">
+        <v>0.46221314622956378</v>
+      </c>
+      <c r="G22" s="85">
+        <v>0.17095594914778819</v>
+      </c>
+      <c r="H22" s="85">
+        <v>-9.7651533876473781E-2</v>
+      </c>
+      <c r="I22" s="85">
+        <v>-0.12945252681650973</v>
+      </c>
+      <c r="J22" s="85">
+        <v>-0.16682497990664674</v>
+      </c>
+      <c r="K22" s="85">
+        <v>0.75679938754267162</v>
+      </c>
+      <c r="L22" s="85">
+        <v>0.28988744818847967</v>
+      </c>
+      <c r="M22" s="85">
+        <v>-0.12730765766412053</v>
+      </c>
+      <c r="N22" s="85">
+        <v>-5.1107312306118231E-16</v>
+      </c>
+      <c r="O22" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P22" s="85">
+        <v>0.38961465936441286</v>
+      </c>
+      <c r="Q22" s="85">
+        <v>0.38622228351709892</v>
+      </c>
+      <c r="R22" s="85">
+        <v>0.27418697316217144</v>
+      </c>
+      <c r="S22" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T22" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U22" s="85">
+        <v>0.44233475653467785</v>
+      </c>
+      <c r="V22" s="85">
+        <v>1</v>
+      </c>
+      <c r="W22" s="85"/>
+      <c r="X22" s="85"/>
+      <c r="Y22" s="85"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="85" t="s">
         <v>93</v>
       </c>
-      <c r="X1" s="72" t="s">
+      <c r="B23" s="85">
+        <v>-0.21401478203302254</v>
+      </c>
+      <c r="C23" s="85">
+        <v>0.6198960282048539</v>
+      </c>
+      <c r="D23" s="85">
+        <v>-0.6186315194591987</v>
+      </c>
+      <c r="E23" s="85">
+        <v>0.48946860211463999</v>
+      </c>
+      <c r="F23" s="85">
+        <v>-0.48615421148870491</v>
+      </c>
+      <c r="G23" s="85">
+        <v>0.12338455418429231</v>
+      </c>
+      <c r="H23" s="85">
+        <v>-6.5234209302127172E-2</v>
+      </c>
+      <c r="I23" s="85">
+        <v>-6.5234209302127172E-2</v>
+      </c>
+      <c r="J23" s="85">
+        <v>8.9003793955071492E-2</v>
+      </c>
+      <c r="K23" s="85">
+        <v>-4.5466267089361322E-2</v>
+      </c>
+      <c r="L23" s="85">
+        <v>2.8057724431021706E-3</v>
+      </c>
+      <c r="M23" s="85">
+        <v>0.29692043293801551</v>
+      </c>
+      <c r="N23" s="85">
+        <v>-1.4953176328571059E-15</v>
+      </c>
+      <c r="O23" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P23" s="85">
+        <v>-0.12444351312777445</v>
+      </c>
+      <c r="Q23" s="85">
+        <v>-0.12335998313694138</v>
+      </c>
+      <c r="R23" s="85">
+        <v>-0.48061968577835246</v>
+      </c>
+      <c r="S23" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T23" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U23" s="85">
+        <v>-0.22700623618415558</v>
+      </c>
+      <c r="V23" s="85">
+        <v>-1.911066179871496E-2</v>
+      </c>
+      <c r="W23" s="85">
+        <v>1</v>
+      </c>
+      <c r="X23" s="85"/>
+      <c r="Y23" s="85"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="85" t="s">
         <v>94</v>
       </c>
-      <c r="Y1" s="72" t="s">
+      <c r="B24" s="85">
+        <v>0.88528380522770744</v>
+      </c>
+      <c r="C24" s="85">
+        <v>0.23877755083096783</v>
+      </c>
+      <c r="D24" s="85">
+        <v>-0.26368965366492136</v>
+      </c>
+      <c r="E24" s="85">
+        <v>0.12156889234959198</v>
+      </c>
+      <c r="F24" s="85">
+        <v>-0.28454014655997628</v>
+      </c>
+      <c r="G24" s="85">
+        <v>-0.49782758967774171</v>
+      </c>
+      <c r="H24" s="85">
+        <v>9.1766396712619255E-2</v>
+      </c>
+      <c r="I24" s="85">
+        <v>0.20604153224154134</v>
+      </c>
+      <c r="J24" s="85">
+        <v>2.501292668571123E-3</v>
+      </c>
+      <c r="K24" s="85">
+        <v>-0.24240180263710734</v>
+      </c>
+      <c r="L24" s="85">
+        <v>-0.44950454092705999</v>
+      </c>
+      <c r="M24" s="85">
+        <v>-9.4570075977804618E-2</v>
+      </c>
+      <c r="N24" s="85">
+        <v>-9.7431870026720007E-16</v>
+      </c>
+      <c r="O24" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P24" s="85">
+        <v>-0.48523636547251753</v>
+      </c>
+      <c r="Q24" s="85">
+        <v>-0.48101141118267471</v>
+      </c>
+      <c r="R24" s="85">
+        <v>2.0299948573528733E-2</v>
+      </c>
+      <c r="S24" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T24" s="85" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U24" s="85">
+        <v>-0.46861278010777019</v>
+      </c>
+      <c r="V24" s="85">
+        <v>-0.36164875740461316</v>
+      </c>
+      <c r="W24" s="85">
+        <v>-0.43432737670120619</v>
+      </c>
+      <c r="X24" s="85">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="85"/>
+    </row>
+    <row r="25" spans="1:25" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A25" s="86" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="73">
-        <v>1</v>
-      </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="73"/>
-      <c r="U2" s="73"/>
-      <c r="V2" s="73"/>
-      <c r="W2" s="73"/>
-      <c r="X2" s="73"/>
-      <c r="Y2" s="73"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="73">
-        <v>0.54532269214902873</v>
-      </c>
-      <c r="C3" s="73">
-        <v>1</v>
-      </c>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="73"/>
-      <c r="Q3" s="73"/>
-      <c r="R3" s="73"/>
-      <c r="S3" s="73"/>
-      <c r="T3" s="73"/>
-      <c r="U3" s="73"/>
-      <c r="V3" s="73"/>
-      <c r="W3" s="73"/>
-      <c r="X3" s="73"/>
-      <c r="Y3" s="73"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B4" s="73">
-        <v>-0.5693038369307919</v>
-      </c>
-      <c r="C4" s="73">
-        <v>-0.99796012768573961</v>
-      </c>
-      <c r="D4" s="73">
-        <v>1</v>
-      </c>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="73"/>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="73"/>
-      <c r="R4" s="73"/>
-      <c r="S4" s="73"/>
-      <c r="T4" s="73"/>
-      <c r="U4" s="73"/>
-      <c r="V4" s="73"/>
-      <c r="W4" s="73"/>
-      <c r="X4" s="73"/>
-      <c r="Y4" s="73"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5" s="73">
-        <v>0.37186951414850039</v>
-      </c>
-      <c r="C5" s="73">
-        <v>0.78685883447847571</v>
-      </c>
-      <c r="D5" s="73">
-        <v>-0.78525374292679184</v>
-      </c>
-      <c r="E5" s="73">
-        <v>1</v>
-      </c>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="73"/>
-      <c r="M5" s="73"/>
-      <c r="N5" s="73"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="73"/>
-      <c r="Q5" s="73"/>
-      <c r="R5" s="73"/>
-      <c r="S5" s="73"/>
-      <c r="T5" s="73"/>
-      <c r="U5" s="73"/>
-      <c r="V5" s="73"/>
-      <c r="W5" s="73"/>
-      <c r="X5" s="73"/>
-      <c r="Y5" s="73"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B6" s="73">
-        <v>-0.52142976010762865</v>
-      </c>
-      <c r="C6" s="73">
-        <v>-0.80214333130506021</v>
-      </c>
-      <c r="D6" s="73">
-        <v>0.80050706133146232</v>
-      </c>
-      <c r="E6" s="73">
-        <v>-0.81378476241257014</v>
-      </c>
-      <c r="F6" s="73">
-        <v>1</v>
-      </c>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="73"/>
-      <c r="N6" s="73"/>
-      <c r="O6" s="73"/>
-      <c r="P6" s="73"/>
-      <c r="Q6" s="73"/>
-      <c r="R6" s="73"/>
-      <c r="S6" s="73"/>
-      <c r="T6" s="73"/>
-      <c r="U6" s="73"/>
-      <c r="V6" s="73"/>
-      <c r="W6" s="73"/>
-      <c r="X6" s="73"/>
-      <c r="Y6" s="73"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B7" s="73">
-        <v>-0.40937219968250366</v>
-      </c>
-      <c r="C7" s="73">
-        <v>-0.24062558079337174</v>
-      </c>
-      <c r="D7" s="73">
-        <v>0.24013473533300858</v>
-      </c>
-      <c r="E7" s="73">
-        <v>-0.17615657920993991</v>
-      </c>
-      <c r="F7" s="73">
-        <v>0.21844348946250985</v>
-      </c>
-      <c r="G7" s="73">
-        <v>1</v>
-      </c>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="73"/>
-      <c r="M7" s="73"/>
-      <c r="N7" s="73"/>
-      <c r="O7" s="73"/>
-      <c r="P7" s="73"/>
-      <c r="Q7" s="73"/>
-      <c r="R7" s="73"/>
-      <c r="S7" s="73"/>
-      <c r="T7" s="73"/>
-      <c r="U7" s="73"/>
-      <c r="V7" s="73"/>
-      <c r="W7" s="73"/>
-      <c r="X7" s="73"/>
-      <c r="Y7" s="73"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B8" s="73">
-        <v>0.2064701282579329</v>
-      </c>
-      <c r="C8" s="73">
-        <v>0.13363062095621231</v>
-      </c>
-      <c r="D8" s="73">
-        <v>-0.13335803155218626</v>
-      </c>
-      <c r="E8" s="73">
-        <v>9.7827974015615812E-2</v>
-      </c>
-      <c r="F8" s="73">
-        <v>-0.1213118698538683</v>
-      </c>
-      <c r="G8" s="73">
-        <v>-0.59150144445301611</v>
-      </c>
-      <c r="H8" s="73">
-        <v>1</v>
-      </c>
-      <c r="I8" s="73"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73"/>
-      <c r="L8" s="73"/>
-      <c r="M8" s="73"/>
-      <c r="N8" s="73"/>
-      <c r="O8" s="73"/>
-      <c r="P8" s="73"/>
-      <c r="Q8" s="73"/>
-      <c r="R8" s="73"/>
-      <c r="S8" s="73"/>
-      <c r="T8" s="73"/>
-      <c r="U8" s="73"/>
-      <c r="V8" s="73"/>
-      <c r="W8" s="73"/>
-      <c r="X8" s="73"/>
-      <c r="Y8" s="73"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B9" s="73">
-        <v>0.2064701282579329</v>
-      </c>
-      <c r="C9" s="73">
-        <v>0.13363062095621234</v>
-      </c>
-      <c r="D9" s="73">
-        <v>-0.13335803155218626</v>
-      </c>
-      <c r="E9" s="73">
-        <v>9.7827974015615812E-2</v>
-      </c>
-      <c r="F9" s="73">
-        <v>-0.1213118698538683</v>
-      </c>
-      <c r="G9" s="73">
-        <v>-0.59150144445301611</v>
-      </c>
-      <c r="H9" s="73">
-        <v>-3.1250000000000097E-2</v>
-      </c>
-      <c r="I9" s="73">
-        <v>1</v>
-      </c>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
-      <c r="M9" s="73"/>
-      <c r="N9" s="73"/>
-      <c r="O9" s="73"/>
-      <c r="P9" s="73"/>
-      <c r="Q9" s="73"/>
-      <c r="R9" s="73"/>
-      <c r="S9" s="73"/>
-      <c r="T9" s="73"/>
-      <c r="U9" s="73"/>
-      <c r="V9" s="73"/>
-      <c r="W9" s="73"/>
-      <c r="X9" s="73"/>
-      <c r="Y9" s="73"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>104</v>
-      </c>
-      <c r="B10" s="73">
-        <v>4.7941143432472522E-2</v>
-      </c>
-      <c r="C10" s="73">
-        <v>0.1689159811730441</v>
-      </c>
-      <c r="D10" s="73">
-        <v>-0.16857141413961296</v>
-      </c>
-      <c r="E10" s="73">
-        <v>0.15141990995385896</v>
-      </c>
-      <c r="F10" s="73">
-        <v>-0.12657001882882701</v>
-      </c>
-      <c r="G10" s="73">
-        <v>-4.0645506075046016E-2</v>
-      </c>
-      <c r="H10" s="73">
-        <v>2.2572347453581727E-2</v>
-      </c>
-      <c r="I10" s="73">
-        <v>2.2572347453581727E-2</v>
-      </c>
-      <c r="J10" s="73">
-        <v>1</v>
-      </c>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="73"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
-      <c r="R10" s="73"/>
-      <c r="S10" s="73"/>
-      <c r="T10" s="73"/>
-      <c r="U10" s="73"/>
-      <c r="V10" s="73"/>
-      <c r="W10" s="73"/>
-      <c r="X10" s="73"/>
-      <c r="Y10" s="73"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>105</v>
-      </c>
-      <c r="B11" s="73">
-        <v>-0.42354601289696908</v>
-      </c>
-      <c r="C11" s="73">
-        <v>-0.46770717334674256</v>
-      </c>
-      <c r="D11" s="73">
-        <v>0.46675311043265155</v>
-      </c>
-      <c r="E11" s="73">
-        <v>-0.41926274578121053</v>
-      </c>
-      <c r="F11" s="73">
-        <v>0.35045651291117474</v>
-      </c>
-      <c r="G11" s="73">
-        <v>0.11254231022778623</v>
-      </c>
-      <c r="H11" s="73">
-        <v>-6.2500000000000042E-2</v>
-      </c>
-      <c r="I11" s="73">
-        <v>-6.2500000000000042E-2</v>
-      </c>
-      <c r="J11" s="73">
-        <v>-0.7674598134217786</v>
-      </c>
-      <c r="K11" s="73">
-        <v>1</v>
-      </c>
-      <c r="L11" s="73"/>
-      <c r="M11" s="73"/>
-      <c r="N11" s="73"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
-      <c r="R11" s="73"/>
-      <c r="S11" s="73"/>
-      <c r="T11" s="73"/>
-      <c r="U11" s="73"/>
-      <c r="V11" s="73"/>
-      <c r="W11" s="73"/>
-      <c r="X11" s="73"/>
-      <c r="Y11" s="73"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B12" s="73">
-        <v>-0.56094629067505208</v>
-      </c>
-      <c r="C12" s="73">
-        <v>-0.48279450151921821</v>
-      </c>
-      <c r="D12" s="73">
-        <v>0.481809662382092</v>
-      </c>
-      <c r="E12" s="73">
-        <v>-0.3534430028951282</v>
-      </c>
-      <c r="F12" s="73">
-        <v>0.43828804592365272</v>
-      </c>
-      <c r="G12" s="73">
-        <v>0.27591017991328259</v>
-      </c>
-      <c r="H12" s="73">
-        <v>-0.15322580645161285</v>
-      </c>
-      <c r="I12" s="73">
-        <v>-0.15322580645161291</v>
-      </c>
-      <c r="J12" s="73">
-        <v>-8.1551706929069462E-2</v>
-      </c>
-      <c r="K12" s="73">
-        <v>0.22580645161290325</v>
-      </c>
-      <c r="L12" s="73">
-        <v>1</v>
-      </c>
-      <c r="M12" s="73"/>
-      <c r="N12" s="73"/>
-      <c r="O12" s="73"/>
-      <c r="P12" s="73"/>
-      <c r="Q12" s="73"/>
-      <c r="R12" s="73"/>
-      <c r="S12" s="73"/>
-      <c r="T12" s="73"/>
-      <c r="U12" s="73"/>
-      <c r="V12" s="73"/>
-      <c r="W12" s="73"/>
-      <c r="X12" s="73"/>
-      <c r="Y12" s="73"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>107</v>
-      </c>
-      <c r="B13" s="73">
-        <v>5.4122225092713113E-3</v>
-      </c>
-      <c r="C13" s="73">
-        <v>0.22252462162536571</v>
-      </c>
-      <c r="D13" s="73">
-        <v>-0.22207069981047078</v>
-      </c>
-      <c r="E13" s="73">
-        <v>0.1629052738543682</v>
-      </c>
-      <c r="F13" s="73">
-        <v>-0.20201116888279116</v>
-      </c>
-      <c r="G13" s="73">
-        <v>9.3703953559000658E-2</v>
-      </c>
-      <c r="H13" s="73">
-        <v>-5.2038180890226576E-2</v>
-      </c>
-      <c r="I13" s="73">
-        <v>-5.2038180890226576E-2</v>
-      </c>
-      <c r="J13" s="73">
-        <v>3.7587964797009037E-2</v>
-      </c>
-      <c r="K13" s="73">
-        <v>-0.10407636178045325</v>
-      </c>
-      <c r="L13" s="73">
-        <v>-0.6983188145269128</v>
-      </c>
-      <c r="M13" s="73">
-        <v>1</v>
-      </c>
-      <c r="N13" s="73"/>
-      <c r="O13" s="73"/>
-      <c r="P13" s="73"/>
-      <c r="Q13" s="73"/>
-      <c r="R13" s="73"/>
-      <c r="S13" s="73"/>
-      <c r="T13" s="73"/>
-      <c r="U13" s="73"/>
-      <c r="V13" s="73"/>
-      <c r="W13" s="73"/>
-      <c r="X13" s="73"/>
-      <c r="Y13" s="73"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>108</v>
-      </c>
-      <c r="B14" s="73">
-        <v>6.8298341815840067E-15</v>
-      </c>
-      <c r="C14" s="73">
-        <v>1.0443996526137254E-16</v>
-      </c>
-      <c r="D14" s="73">
-        <v>-1.0422692106773353E-16</v>
-      </c>
-      <c r="E14" s="73">
-        <v>1.5603704304785335E-17</v>
-      </c>
-      <c r="F14" s="73">
-        <v>-1.6554503680555037E-16</v>
-      </c>
-      <c r="G14" s="73">
-        <v>2.9587283593366958E-16</v>
-      </c>
-      <c r="H14" s="73">
-        <v>-6.9781887052612257E-17</v>
-      </c>
-      <c r="I14" s="73">
-        <v>-6.9781887052612257E-17</v>
-      </c>
-      <c r="J14" s="73">
-        <v>-2.3690120647793115E-16</v>
-      </c>
-      <c r="K14" s="73">
-        <v>0</v>
-      </c>
-      <c r="L14" s="73">
-        <v>-2.9713577712725213E-16</v>
-      </c>
-      <c r="M14" s="73">
-        <v>1.3072760860698715E-16</v>
-      </c>
-      <c r="N14" s="73">
-        <v>1</v>
-      </c>
-      <c r="O14" s="73"/>
-      <c r="P14" s="73"/>
-      <c r="Q14" s="73"/>
-      <c r="R14" s="73"/>
-      <c r="S14" s="73"/>
-      <c r="T14" s="73"/>
-      <c r="U14" s="73"/>
-      <c r="V14" s="73"/>
-      <c r="W14" s="73"/>
-      <c r="X14" s="73"/>
-      <c r="Y14" s="73"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B15" s="73" t="e">
+      <c r="B25" s="86">
+        <v>-0.53311575526124477</v>
+      </c>
+      <c r="C25" s="86" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="C15" s="73" t="e">
+      <c r="D25" s="86" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="D15" s="73" t="e">
+      <c r="E25" s="86" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="E15" s="73" t="e">
+      <c r="F25" s="86" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="F15" s="73" t="e">
+      <c r="G25" s="86" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="G15" s="73" t="e">
+      <c r="H25" s="86" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="H15" s="73" t="e">
+      <c r="I25" s="86" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="I15" s="73" t="e">
+      <c r="J25" s="86">
+        <v>-0.36806088975493934</v>
+      </c>
+      <c r="K25" s="86">
+        <v>0.66445163137920571</v>
+      </c>
+      <c r="L25" s="86" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="J15" s="73" t="e">
+      <c r="M25" s="86" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="K15" s="73" t="e">
+      <c r="N25" s="86">
+        <v>-2.0100642720231223E-16</v>
+      </c>
+      <c r="O25" s="86" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="L15" s="73" t="e">
+      <c r="P25" s="86" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="M15" s="73" t="e">
+      <c r="Q25" s="86" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="N15" s="73" t="e">
+      <c r="R25" s="86" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="O15" s="73">
-        <v>1</v>
-      </c>
-      <c r="P15" s="73"/>
-      <c r="Q15" s="73"/>
-      <c r="R15" s="73"/>
-      <c r="S15" s="73"/>
-      <c r="T15" s="73"/>
-      <c r="U15" s="73"/>
-      <c r="V15" s="73"/>
-      <c r="W15" s="73"/>
-      <c r="X15" s="73"/>
-      <c r="Y15" s="73"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" s="73">
-        <v>-0.63644724213007908</v>
-      </c>
-      <c r="C16" s="73">
-        <v>-0.64888568452304984</v>
-      </c>
-      <c r="D16" s="73">
-        <v>0.64756204058007127</v>
-      </c>
-      <c r="E16" s="73">
-        <v>-0.47503462477680736</v>
-      </c>
-      <c r="F16" s="73">
-        <v>0.58906809792264891</v>
-      </c>
-      <c r="G16" s="73">
-        <v>0.37082892492880132</v>
-      </c>
-      <c r="H16" s="73">
-        <v>-0.20593861776197844</v>
-      </c>
-      <c r="I16" s="73">
-        <v>-0.20593861776197844</v>
-      </c>
-      <c r="J16" s="73">
-        <v>-0.10960716207035329</v>
-      </c>
-      <c r="K16" s="73">
-        <v>0.30348848933344197</v>
-      </c>
-      <c r="L16" s="73">
-        <v>0.74403629643037428</v>
-      </c>
-      <c r="M16" s="73">
-        <v>-0.34293347338819458</v>
-      </c>
-      <c r="N16" s="73">
-        <v>-2.3598342282655199E-16</v>
-      </c>
-      <c r="O16" s="73" t="e">
+      <c r="S25" s="86" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="P16" s="73">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="73"/>
-      <c r="R16" s="73"/>
-      <c r="S16" s="73"/>
-      <c r="T16" s="73"/>
-      <c r="U16" s="73"/>
-      <c r="V16" s="73"/>
-      <c r="W16" s="73"/>
-      <c r="X16" s="73"/>
-      <c r="Y16" s="73"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" s="73">
-        <v>-0.63090569434588195</v>
-      </c>
-      <c r="C17" s="73">
-        <v>-0.64323583518874972</v>
-      </c>
-      <c r="D17" s="73">
-        <v>0.64192371621700783</v>
-      </c>
-      <c r="E17" s="73">
-        <v>-0.47089849706960152</v>
-      </c>
-      <c r="F17" s="73">
-        <v>0.58393908046967202</v>
-      </c>
-      <c r="G17" s="73">
-        <v>0.3676001165198311</v>
-      </c>
-      <c r="H17" s="73">
-        <v>-0.20414550968420586</v>
-      </c>
-      <c r="I17" s="73">
-        <v>-0.20414550968420586</v>
-      </c>
-      <c r="J17" s="73">
-        <v>-0.10865281222657011</v>
-      </c>
-      <c r="K17" s="73">
-        <v>0.3008460142714614</v>
-      </c>
-      <c r="L17" s="73">
-        <v>0.73755797047197014</v>
-      </c>
-      <c r="M17" s="73">
-        <v>-0.339947550747975</v>
-      </c>
-      <c r="N17" s="73">
-        <v>-2.1497449050234554E-16</v>
-      </c>
-      <c r="O17" s="73" t="e">
+      <c r="T25" s="86" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="P17" s="73">
-        <v>0.99129299741224342</v>
-      </c>
-      <c r="Q17" s="73">
-        <v>1</v>
-      </c>
-      <c r="R17" s="73"/>
-      <c r="S17" s="73"/>
-      <c r="T17" s="73"/>
-      <c r="U17" s="73"/>
-      <c r="V17" s="73"/>
-      <c r="W17" s="73"/>
-      <c r="X17" s="73"/>
-      <c r="Y17" s="73"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>89</v>
-      </c>
-      <c r="B18" s="73">
-        <v>-0.26911365410861021</v>
-      </c>
-      <c r="C18" s="73">
-        <v>-0.30860669992418377</v>
-      </c>
-      <c r="D18" s="73">
-        <v>0.30752176228926043</v>
-      </c>
-      <c r="E18" s="73">
-        <v>6.976819652324362E-2</v>
-      </c>
-      <c r="F18" s="73">
-        <v>0.26379467179224692</v>
-      </c>
-      <c r="G18" s="73" t="e">
+      <c r="U25" s="86" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="H18" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I18" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J18" s="73">
-        <v>-3.9904344223381058E-2</v>
-      </c>
-      <c r="K18" s="73">
-        <v>0.11526067913468739</v>
-      </c>
-      <c r="L18" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M18" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N18" s="73">
-        <v>1.6764008022404885E-15</v>
-      </c>
-      <c r="O18" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P18" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q18" s="73">
-        <v>0</v>
-      </c>
-      <c r="R18" s="73">
-        <v>1</v>
-      </c>
-      <c r="S18" s="73"/>
-      <c r="T18" s="73"/>
-      <c r="U18" s="73"/>
-      <c r="V18" s="73"/>
-      <c r="W18" s="73"/>
-      <c r="X18" s="73"/>
-      <c r="Y18" s="73"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B19" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C19" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D19" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E19" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F19" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G19" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H19" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I19" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J19" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K19" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L19" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M19" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N19" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O19" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P19" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q19" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R19" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S19" s="73">
-        <v>1</v>
-      </c>
-      <c r="T19" s="73"/>
-      <c r="U19" s="73"/>
-      <c r="V19" s="73"/>
-      <c r="W19" s="73"/>
-      <c r="X19" s="73"/>
-      <c r="Y19" s="73"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C20" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D20" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E20" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F20" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G20" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H20" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I20" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J20" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K20" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L20" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M20" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N20" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O20" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P20" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q20" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R20" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S20" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T20" s="73">
-        <v>1</v>
-      </c>
-      <c r="U20" s="73"/>
-      <c r="V20" s="73"/>
-      <c r="W20" s="73"/>
-      <c r="X20" s="73"/>
-      <c r="Y20" s="73"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
-        <v>122</v>
-      </c>
-      <c r="B21" s="73">
-        <v>-0.65684655212468779</v>
-      </c>
-      <c r="C21" s="73">
-        <v>-0.74501977471698688</v>
-      </c>
-      <c r="D21" s="73">
-        <v>0.74350002950496497</v>
-      </c>
-      <c r="E21" s="73">
-        <v>-0.54541223142273476</v>
-      </c>
-      <c r="F21" s="73">
-        <v>0.67634005815658671</v>
-      </c>
-      <c r="G21" s="73">
-        <v>0.30504180067972075</v>
-      </c>
-      <c r="H21" s="73">
-        <v>-0.15636742794798861</v>
-      </c>
-      <c r="I21" s="73">
-        <v>-0.15636742794798861</v>
-      </c>
-      <c r="J21" s="73">
-        <v>-0.12584574623964012</v>
-      </c>
-      <c r="K21" s="73">
-        <v>0.34845109292030901</v>
-      </c>
-      <c r="L21" s="73">
-        <v>0.76338890244138069</v>
-      </c>
-      <c r="M21" s="73">
-        <v>-0.38484971956554048</v>
-      </c>
-      <c r="N21" s="73">
-        <v>2.2613484572857596E-16</v>
-      </c>
-      <c r="O21" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P21" s="73">
-        <v>0.78920382806196909</v>
-      </c>
-      <c r="Q21" s="73">
-        <v>0.79023941466963321</v>
-      </c>
-      <c r="R21" s="73">
-        <v>0.86221131987965471</v>
-      </c>
-      <c r="S21" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T21" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U21" s="73">
-        <v>1</v>
-      </c>
-      <c r="V21" s="73"/>
-      <c r="W21" s="73"/>
-      <c r="X21" s="73"/>
-      <c r="Y21" s="73"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
-        <v>92</v>
-      </c>
-      <c r="B22" s="73">
-        <v>-0.6139086961176804</v>
-      </c>
-      <c r="C22" s="73">
-        <v>-0.5947704002421923</v>
-      </c>
-      <c r="D22" s="73">
-        <v>0.59355714456939646</v>
-      </c>
-      <c r="E22" s="73">
-        <v>-0.55235314072510733</v>
-      </c>
-      <c r="F22" s="73">
-        <v>0.46221314622956378</v>
-      </c>
-      <c r="G22" s="73">
-        <v>0.17095594914778819</v>
-      </c>
-      <c r="H22" s="73">
-        <v>-9.7651533876473781E-2</v>
-      </c>
-      <c r="I22" s="73">
-        <v>-0.12945252681650973</v>
-      </c>
-      <c r="J22" s="73">
-        <v>-0.16682497990664674</v>
-      </c>
-      <c r="K22" s="73">
-        <v>0.75679938754267162</v>
-      </c>
-      <c r="L22" s="73">
-        <v>0.28988744818847967</v>
-      </c>
-      <c r="M22" s="73">
-        <v>-0.12730765766412053</v>
-      </c>
-      <c r="N22" s="73">
-        <v>-5.1107312306118231E-16</v>
-      </c>
-      <c r="O22" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P22" s="73">
-        <v>0.38961465936441286</v>
-      </c>
-      <c r="Q22" s="73">
-        <v>0.38622228351709892</v>
-      </c>
-      <c r="R22" s="73">
-        <v>0.13174403224453668</v>
-      </c>
-      <c r="S22" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T22" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U22" s="73">
-        <v>0.44233475653467785</v>
-      </c>
-      <c r="V22" s="73">
-        <v>1</v>
-      </c>
-      <c r="W22" s="73"/>
-      <c r="X22" s="73"/>
-      <c r="Y22" s="73"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
-        <v>93</v>
-      </c>
-      <c r="B23" s="73">
-        <v>-0.21401478203302254</v>
-      </c>
-      <c r="C23" s="73">
-        <v>0.6198960282048539</v>
-      </c>
-      <c r="D23" s="73">
-        <v>-0.6186315194591987</v>
-      </c>
-      <c r="E23" s="73">
-        <v>0.48946860211463999</v>
-      </c>
-      <c r="F23" s="73">
-        <v>-0.48615421148870491</v>
-      </c>
-      <c r="G23" s="73">
-        <v>0.12338455418429231</v>
-      </c>
-      <c r="H23" s="73">
-        <v>-6.5234209302127172E-2</v>
-      </c>
-      <c r="I23" s="73">
-        <v>-6.5234209302127172E-2</v>
-      </c>
-      <c r="J23" s="73">
-        <v>8.9003793955071492E-2</v>
-      </c>
-      <c r="K23" s="73">
-        <v>-4.5466267089361322E-2</v>
-      </c>
-      <c r="L23" s="73">
-        <v>2.8057724431021706E-3</v>
-      </c>
-      <c r="M23" s="73">
-        <v>0.29692043293801551</v>
-      </c>
-      <c r="N23" s="73">
-        <v>-1.4953176328571059E-15</v>
-      </c>
-      <c r="O23" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P23" s="73">
-        <v>-0.12444351312777445</v>
-      </c>
-      <c r="Q23" s="73">
-        <v>-0.12335998313694138</v>
-      </c>
-      <c r="R23" s="73">
-        <v>-0.2483609982908293</v>
-      </c>
-      <c r="S23" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T23" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U23" s="73">
-        <v>-0.22700623618415558</v>
-      </c>
-      <c r="V23" s="73">
-        <v>-1.911066179871496E-2</v>
-      </c>
-      <c r="W23" s="73">
-        <v>1</v>
-      </c>
-      <c r="X23" s="73"/>
-      <c r="Y23" s="73"/>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
-        <v>94</v>
-      </c>
-      <c r="B24" s="73">
-        <v>0.88528380522770744</v>
-      </c>
-      <c r="C24" s="73">
-        <v>0.23877755083096783</v>
-      </c>
-      <c r="D24" s="73">
-        <v>-0.26368965366492136</v>
-      </c>
-      <c r="E24" s="73">
-        <v>0.12156889234959198</v>
-      </c>
-      <c r="F24" s="73">
-        <v>-0.28454014655997628</v>
-      </c>
-      <c r="G24" s="73">
-        <v>-0.49782758967774171</v>
-      </c>
-      <c r="H24" s="73">
-        <v>9.1766396712619255E-2</v>
-      </c>
-      <c r="I24" s="73">
-        <v>0.20604153224154134</v>
-      </c>
-      <c r="J24" s="73">
-        <v>2.501292668571123E-3</v>
-      </c>
-      <c r="K24" s="73">
-        <v>-0.24240180263710734</v>
-      </c>
-      <c r="L24" s="73">
-        <v>-0.44950454092705999</v>
-      </c>
-      <c r="M24" s="73">
-        <v>-9.4570075977804618E-2</v>
-      </c>
-      <c r="N24" s="73">
-        <v>-9.7431870026720007E-16</v>
-      </c>
-      <c r="O24" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P24" s="73">
-        <v>-0.48523636547251753</v>
-      </c>
-      <c r="Q24" s="73">
-        <v>-0.48101141118267471</v>
-      </c>
-      <c r="R24" s="73">
-        <v>-0.14641107432910491</v>
-      </c>
-      <c r="S24" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T24" s="73" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U24" s="73">
-        <v>-0.46861278010777019</v>
-      </c>
-      <c r="V24" s="73">
-        <v>-0.36164875740461316</v>
-      </c>
-      <c r="W24" s="73">
-        <v>-0.43432737670120619</v>
-      </c>
-      <c r="X24" s="73">
-        <v>1</v>
-      </c>
-      <c r="Y24" s="73"/>
-    </row>
-    <row r="25" spans="1:25" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A25" s="71" t="s">
-        <v>95</v>
-      </c>
-      <c r="B25" s="74">
-        <v>-0.53311575526124477</v>
-      </c>
-      <c r="C25" s="74" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D25" s="74" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E25" s="74" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F25" s="74" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G25" s="74" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H25" s="74" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I25" s="74" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J25" s="74">
-        <v>-0.36806088975493934</v>
-      </c>
-      <c r="K25" s="74">
-        <v>0.66445163137920571</v>
-      </c>
-      <c r="L25" s="74" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M25" s="74" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N25" s="74">
-        <v>-2.0100642720231223E-16</v>
-      </c>
-      <c r="O25" s="74" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P25" s="74" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q25" s="74" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R25" s="74" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S25" s="74" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T25" s="74" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U25" s="74" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V25" s="74">
+      <c r="V25" s="86">
         <v>0.63089909132674227</v>
       </c>
-      <c r="W25" s="74">
+      <c r="W25" s="86">
         <v>0.59991265498140522</v>
       </c>
-      <c r="X25" s="74">
+      <c r="X25" s="86">
         <v>-0.53311575526124488</v>
       </c>
-      <c r="Y25" s="74">
+      <c r="Y25" s="86">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="A1:Y25">
+  <conditionalFormatting sqref="B2:Y25">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -18654,9 +18670,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFD9269-7F18-4E64-8D48-3C1F1E4D91C0}">
   <dimension ref="B2:AF47"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+    <sheetView showGridLines="0" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="5" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V26" sqref="V26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -20840,7 +20856,7 @@
         <v>100</v>
       </c>
       <c r="V25" s="1">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="W25" s="1">
         <v>10</v>
@@ -22406,15 +22422,15 @@
       <c r="Z42" s="55">
         <v>2</v>
       </c>
-      <c r="AA42" s="75">
+      <c r="AA42" s="71">
         <f t="shared" si="13"/>
         <v>5</v>
       </c>
-      <c r="AB42" s="76">
+      <c r="AB42" s="72">
         <f t="shared" si="14"/>
         <v>1.46</v>
       </c>
-      <c r="AC42" s="75">
+      <c r="AC42" s="71">
         <f t="shared" si="15"/>
         <v>9.1999999999999993</v>
       </c>
@@ -22422,7 +22438,7 @@
         <f t="shared" si="16"/>
         <v>34</v>
       </c>
-      <c r="AE42" s="75">
+      <c r="AE42" s="71">
         <f t="shared" si="17"/>
         <v>11.6</v>
       </c>
@@ -22499,15 +22515,15 @@
       <c r="Z43" s="55">
         <v>2</v>
       </c>
-      <c r="AA43" s="75">
+      <c r="AA43" s="71">
         <f t="shared" si="13"/>
         <v>5</v>
       </c>
-      <c r="AB43" s="76">
+      <c r="AB43" s="72">
         <f t="shared" si="14"/>
         <v>1.43</v>
       </c>
-      <c r="AC43" s="75">
+      <c r="AC43" s="71">
         <f t="shared" si="15"/>
         <v>9.1</v>
       </c>
@@ -22515,7 +22531,7 @@
         <f t="shared" si="16"/>
         <v>34</v>
       </c>
-      <c r="AE43" s="75">
+      <c r="AE43" s="71">
         <f t="shared" si="17"/>
         <v>11.5</v>
       </c>
@@ -22592,15 +22608,15 @@
       <c r="Z44" s="55">
         <v>2</v>
       </c>
-      <c r="AA44" s="75">
+      <c r="AA44" s="71">
         <f t="shared" si="13"/>
         <v>5</v>
       </c>
-      <c r="AB44" s="76">
+      <c r="AB44" s="72">
         <f t="shared" si="14"/>
         <v>1.41</v>
       </c>
-      <c r="AC44" s="75">
+      <c r="AC44" s="71">
         <f t="shared" si="15"/>
         <v>9</v>
       </c>
@@ -22608,7 +22624,7 @@
         <f t="shared" si="16"/>
         <v>34</v>
       </c>
-      <c r="AE44" s="75">
+      <c r="AE44" s="71">
         <f t="shared" si="17"/>
         <v>11.4</v>
       </c>

</xml_diff>